<commit_message>
:construction: field 정렬 옵션 추가. ExcelColumn 의 value 가 empty string 인 경우 필드명으로 출력 처리
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -232,54 +232,54 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>foo</t>
+          <t>aaaa</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>bar</t>
+          <t>bbbb</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>블라블라?블~라~블~라~</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>가</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>블라블라?블~라~블~라~</t>
-        </is>
-      </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>다</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>https://www.google.com</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>바</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>https://www.google.com</t>
         </is>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
:construction: ExcelStyle dataFormat 옵션 추가
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -232,54 +232,90 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>aaaa</t>
+          <t>a푸</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>bbbb</t>
+          <t>b파</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>cost</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>가</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>블라블라?블~라~블~라~</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>가</t>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t/>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>나</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>다</t>
         </is>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>https://www.google.com</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>바</t>
-        </is>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>라</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>https://www.naver.com</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>100000.0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
:construction: class 기반 style 기능 추가
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -37,24 +37,11 @@
       <name val="Calibri"/>
       <sz val="11.0"/>
       <color indexed="8"/>
-      <i val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
       <b val="true"/>
       <u val="none"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-      <u val="none"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -73,6 +60,11 @@
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
       </patternFill>
     </fill>
     <fill>
@@ -217,15 +209,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
       <alignment shrinkToFit="false" horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
       <alignment shrinkToFit="false" horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment shrinkToFit="false" horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true">
-      <alignment shrinkToFit="false" horizontal="general" vertical="bottom"/>
-    </xf>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>

</xml_diff>

<commit_message>
:construction: type 타입 체킹 수정
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -204,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
       <alignment shrinkToFit="false" horizontal="general" vertical="bottom"/>
@@ -214,7 +214,8 @@
       <alignment shrinkToFit="false" horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -243,6 +244,11 @@
           <t>비용</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>비용xxxxxxx</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -260,6 +266,9 @@
           <t/>
         </is>
       </c>
+      <c r="D2" s="6" t="n">
+        <v>0.10000000149011612</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
@@ -277,6 +286,9 @@
           <t/>
         </is>
       </c>
+      <c r="D3" s="6" t="n">
+        <v>0.10000000149011612</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
@@ -294,6 +306,9 @@
           <t/>
         </is>
       </c>
+      <c r="D4" s="6" t="n">
+        <v>0.10000000149011612</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
@@ -308,6 +323,9 @@
       </c>
       <c r="C5" s="5" t="n">
         <v>100000.0</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>0.10000000149011612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:construction: @ExcelStyle 속성 추가
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -208,12 +208,12 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment shrinkToFit="false" horizontal="general" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true" quotePrefix="false">
+      <alignment horizontal="general" vertical="bottom" shrinkToFit="false" wrapText="false" textRotation="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="164" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true">
-      <alignment shrinkToFit="false" horizontal="general" vertical="bottom"/>
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true" quotePrefix="false" applyNumberFormat="true">
+      <alignment horizontal="general" vertical="bottom" shrinkToFit="false" wrapText="false" textRotation="0"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyNumberFormat="true"/>
@@ -270,13 +270,13 @@
         </is>
       </c>
       <c r="C2" s="5" t="n">
-        <v>881023.0</v>
+        <v>760919.0</v>
       </c>
       <c r="D2" s="6" t="n">
-        <v>920019.1875</v>
+        <v>560638.3125</v>
       </c>
       <c r="E2" s="7" t="n">
-        <v>659532.0</v>
+        <v>35489.0</v>
       </c>
     </row>
     <row r="3">
@@ -291,13 +291,13 @@
         </is>
       </c>
       <c r="C3" s="5" t="n">
-        <v>455788.0</v>
+        <v>443485.0</v>
       </c>
       <c r="D3" s="6" t="n">
-        <v>221671.046875</v>
+        <v>586050.6875</v>
       </c>
       <c r="E3" s="7" t="n">
-        <v>626754.0</v>
+        <v>39459.0</v>
       </c>
     </row>
     <row r="4">
@@ -312,13 +312,13 @@
         </is>
       </c>
       <c r="C4" s="5" t="n">
-        <v>89370.0</v>
+        <v>932822.0</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>713732.375</v>
+        <v>934342.625</v>
       </c>
       <c r="E4" s="7" t="n">
-        <v>695675.0</v>
+        <v>233926.0</v>
       </c>
     </row>
     <row r="5">
@@ -333,13 +333,13 @@
         </is>
       </c>
       <c r="C5" s="5" t="n">
-        <v>454677.0</v>
+        <v>87801.0</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>557897.8125</v>
+        <v>566185.0</v>
       </c>
       <c r="E5" s="7" t="n">
-        <v>600478.0</v>
+        <v>73175.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:sparkles: #2 컬럼 width 설정 옵션 추가
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -17,8 +17,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode=""/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd hh:mm:ss"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -206,19 +207,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true" quotePrefix="false">
       <alignment horizontal="general" vertical="bottom" shrinkToFit="false" wrapText="false" textRotation="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="164" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true" quotePrefix="false" applyNumberFormat="true">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true" quotePrefix="false" applyNumberFormat="true">
       <alignment horizontal="general" vertical="bottom" shrinkToFit="false" wrapText="false" textRotation="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="4" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -233,6 +237,16 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="8" customHeight="true"/>
+  <cols>
+    <col min="1" max="1" width="8.0" customWidth="true"/>
+    <col min="2" max="2" width="8.0" customWidth="true"/>
+    <col min="3" max="3" width="8.0" customWidth="true"/>
+    <col min="4" max="4" width="8.0" customWidth="true"/>
+    <col min="5" max="5" width="8.0" customWidth="true"/>
+    <col min="6" max="6" width="8.0" customWidth="true"/>
+    <col min="7" max="7" width="16.0" customWidth="true"/>
+    <col min="8" max="8" width="8.0" customWidth="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -260,6 +274,21 @@
           <t>long~~~~</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>date2</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>dateTime</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -273,13 +302,22 @@
         </is>
       </c>
       <c r="C2" s="5" t="n">
-        <v>36802.0</v>
+        <v>946554.0</v>
       </c>
       <c r="D2" s="6" t="n">
-        <v>928899.75</v>
+        <v>915719.8125</v>
       </c>
       <c r="E2" s="7" t="n">
-        <v>263506.0</v>
+        <v>198620.0</v>
+      </c>
+      <c r="F2" s="8" t="n">
+        <v>45020.0</v>
+      </c>
+      <c r="G2" s="9" t="n">
+        <v>45020.68039681713</v>
+      </c>
+      <c r="H2" s="10" t="n">
+        <v>45020.68039681713</v>
       </c>
     </row>
     <row r="3">
@@ -294,13 +332,22 @@
         </is>
       </c>
       <c r="C3" s="5" t="n">
-        <v>626875.0</v>
+        <v>159781.0</v>
       </c>
       <c r="D3" s="6" t="n">
-        <v>591513.9375</v>
+        <v>865246.5</v>
       </c>
       <c r="E3" s="7" t="n">
-        <v>185492.0</v>
+        <v>778848.0</v>
+      </c>
+      <c r="F3" s="8" t="n">
+        <v>45020.0</v>
+      </c>
+      <c r="G3" s="9" t="n">
+        <v>45020.68039681713</v>
+      </c>
+      <c r="H3" s="10" t="n">
+        <v>45020.68039681713</v>
       </c>
     </row>
     <row r="4">
@@ -315,13 +362,22 @@
         </is>
       </c>
       <c r="C4" s="5" t="n">
-        <v>831560.0</v>
+        <v>375230.0</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>317807.1875</v>
+        <v>927798.1875</v>
       </c>
       <c r="E4" s="7" t="n">
-        <v>79913.0</v>
+        <v>438320.0</v>
+      </c>
+      <c r="F4" s="8" t="n">
+        <v>45020.0</v>
+      </c>
+      <c r="G4" s="9" t="n">
+        <v>45020.68039681713</v>
+      </c>
+      <c r="H4" s="10" t="n">
+        <v>45020.68039681713</v>
       </c>
     </row>
     <row r="5">
@@ -336,13 +392,22 @@
         </is>
       </c>
       <c r="C5" s="5" t="n">
-        <v>953130.0</v>
+        <v>809286.0</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>438784.90625</v>
+        <v>313665.15625</v>
       </c>
       <c r="E5" s="7" t="n">
-        <v>204136.0</v>
+        <v>247158.0</v>
+      </c>
+      <c r="F5" s="8" t="n">
+        <v>45020.0</v>
+      </c>
+      <c r="G5" s="9" t="n">
+        <v>45020.68039681713</v>
+      </c>
+      <c r="H5" s="10" t="n">
+        <v>45020.68039681713</v>
       </c>
     </row>
     <row r="6">
@@ -357,13 +422,22 @@
         </is>
       </c>
       <c r="C6" s="5" t="n">
-        <v>429631.0</v>
+        <v>502536.0</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>613835.0625</v>
+        <v>427313.6875</v>
       </c>
       <c r="E6" s="7" t="n">
-        <v>201256.0</v>
+        <v>297902.0</v>
+      </c>
+      <c r="F6" s="8" t="n">
+        <v>45020.0</v>
+      </c>
+      <c r="G6" s="9" t="n">
+        <v>45020.68039681713</v>
+      </c>
+      <c r="H6" s="10" t="n">
+        <v>45020.68039681713</v>
       </c>
     </row>
     <row r="7">
@@ -378,13 +452,22 @@
         </is>
       </c>
       <c r="C7" s="5" t="n">
-        <v>388435.0</v>
+        <v>755012.0</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>873887.3125</v>
+        <v>9438.6337890625</v>
       </c>
       <c r="E7" s="7" t="n">
-        <v>433217.0</v>
+        <v>359439.0</v>
+      </c>
+      <c r="F7" s="8" t="n">
+        <v>45020.0</v>
+      </c>
+      <c r="G7" s="9" t="n">
+        <v>45020.68039681713</v>
+      </c>
+      <c r="H7" s="10" t="n">
+        <v>45020.68039681713</v>
       </c>
     </row>
     <row r="8">
@@ -399,13 +482,22 @@
         </is>
       </c>
       <c r="C8" s="5" t="n">
-        <v>717184.0</v>
+        <v>277095.0</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>762926.25</v>
+        <v>198209.9375</v>
       </c>
       <c r="E8" s="7" t="n">
-        <v>26205.0</v>
+        <v>742489.0</v>
+      </c>
+      <c r="F8" s="8" t="n">
+        <v>45020.0</v>
+      </c>
+      <c r="G8" s="9" t="n">
+        <v>45020.68039681713</v>
+      </c>
+      <c r="H8" s="10" t="n">
+        <v>45020.68039681713</v>
       </c>
     </row>
     <row r="9">
@@ -420,13 +512,22 @@
         </is>
       </c>
       <c r="C9" s="5" t="n">
-        <v>168323.0</v>
+        <v>833938.0</v>
       </c>
       <c r="D9" s="6" t="n">
-        <v>532343.1875</v>
+        <v>904344.6875</v>
       </c>
       <c r="E9" s="7" t="n">
-        <v>54946.0</v>
+        <v>784051.0</v>
+      </c>
+      <c r="F9" s="8" t="n">
+        <v>45020.0</v>
+      </c>
+      <c r="G9" s="9" t="n">
+        <v>45020.68039681713</v>
+      </c>
+      <c r="H9" s="10" t="n">
+        <v>45020.68039681713</v>
       </c>
     </row>
     <row r="10">
@@ -441,13 +542,22 @@
         </is>
       </c>
       <c r="C10" s="5" t="n">
-        <v>952127.0</v>
+        <v>428110.0</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>201007.3125</v>
+        <v>763257.5</v>
       </c>
       <c r="E10" s="7" t="n">
-        <v>387339.0</v>
+        <v>552668.0</v>
+      </c>
+      <c r="F10" s="8" t="n">
+        <v>45020.0</v>
+      </c>
+      <c r="G10" s="9" t="n">
+        <v>45020.68039681713</v>
+      </c>
+      <c r="H10" s="10" t="n">
+        <v>45020.68039681713</v>
       </c>
     </row>
     <row r="11">
@@ -462,13 +572,22 @@
         </is>
       </c>
       <c r="C11" s="5" t="n">
-        <v>868548.0</v>
+        <v>183983.0</v>
       </c>
       <c r="D11" s="6" t="n">
-        <v>601624.875</v>
+        <v>813212.0625</v>
       </c>
       <c r="E11" s="7" t="n">
-        <v>503445.0</v>
+        <v>24319.0</v>
+      </c>
+      <c r="F11" s="8" t="n">
+        <v>45020.0</v>
+      </c>
+      <c r="G11" s="9" t="n">
+        <v>45020.68039681713</v>
+      </c>
+      <c r="H11" s="10" t="n">
+        <v>45020.68039681713</v>
       </c>
     </row>
     <row r="12">
@@ -483,13 +602,22 @@
         </is>
       </c>
       <c r="C12" s="5" t="n">
-        <v>520373.0</v>
+        <v>652746.0</v>
       </c>
       <c r="D12" s="6" t="n">
-        <v>994859.625</v>
+        <v>247624.34375</v>
       </c>
       <c r="E12" s="7" t="n">
-        <v>835985.0</v>
+        <v>164234.0</v>
+      </c>
+      <c r="F12" s="8" t="n">
+        <v>45020.0</v>
+      </c>
+      <c r="G12" s="9" t="n">
+        <v>45020.68039681713</v>
+      </c>
+      <c r="H12" s="10" t="n">
+        <v>45020.68039681713</v>
       </c>
     </row>
     <row r="13">
@@ -504,13 +632,22 @@
         </is>
       </c>
       <c r="C13" s="5" t="n">
-        <v>77652.0</v>
+        <v>326721.0</v>
       </c>
       <c r="D13" s="6" t="n">
-        <v>756790.3125</v>
+        <v>254885.375</v>
       </c>
       <c r="E13" s="7" t="n">
-        <v>890309.0</v>
+        <v>944602.0</v>
+      </c>
+      <c r="F13" s="8" t="n">
+        <v>45020.0</v>
+      </c>
+      <c r="G13" s="9" t="n">
+        <v>45020.68039681713</v>
+      </c>
+      <c r="H13" s="10" t="n">
+        <v>45020.68039681713</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:sparkles: #2 컬럼 auto width 설정 옵션 추가
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -302,22 +302,22 @@
         </is>
       </c>
       <c r="C2" s="5" t="n">
-        <v>946554.0</v>
+        <v>922319.0</v>
       </c>
       <c r="D2" s="6" t="n">
-        <v>915719.8125</v>
+        <v>415785.1875</v>
       </c>
       <c r="E2" s="7" t="n">
-        <v>198620.0</v>
+        <v>975595.0</v>
       </c>
       <c r="F2" s="8" t="n">
         <v>45020.0</v>
       </c>
       <c r="G2" s="9" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
       <c r="H2" s="10" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
     </row>
     <row r="3">
@@ -332,22 +332,22 @@
         </is>
       </c>
       <c r="C3" s="5" t="n">
-        <v>159781.0</v>
+        <v>476448.0</v>
       </c>
       <c r="D3" s="6" t="n">
-        <v>865246.5</v>
+        <v>652313.1875</v>
       </c>
       <c r="E3" s="7" t="n">
-        <v>778848.0</v>
+        <v>742906.0</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>45020.0</v>
       </c>
       <c r="G3" s="9" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
       <c r="H3" s="10" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
     </row>
     <row r="4">
@@ -362,22 +362,22 @@
         </is>
       </c>
       <c r="C4" s="5" t="n">
-        <v>375230.0</v>
+        <v>373542.0</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>927798.1875</v>
+        <v>430267.40625</v>
       </c>
       <c r="E4" s="7" t="n">
-        <v>438320.0</v>
+        <v>39273.0</v>
       </c>
       <c r="F4" s="8" t="n">
         <v>45020.0</v>
       </c>
       <c r="G4" s="9" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
       <c r="H4" s="10" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
     </row>
     <row r="5">
@@ -392,22 +392,22 @@
         </is>
       </c>
       <c r="C5" s="5" t="n">
-        <v>809286.0</v>
+        <v>864392.0</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>313665.15625</v>
+        <v>820477.75</v>
       </c>
       <c r="E5" s="7" t="n">
-        <v>247158.0</v>
+        <v>896935.0</v>
       </c>
       <c r="F5" s="8" t="n">
         <v>45020.0</v>
       </c>
       <c r="G5" s="9" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
       <c r="H5" s="10" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
     </row>
     <row r="6">
@@ -422,22 +422,22 @@
         </is>
       </c>
       <c r="C6" s="5" t="n">
-        <v>502536.0</v>
+        <v>970491.0</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>427313.6875</v>
+        <v>725982.875</v>
       </c>
       <c r="E6" s="7" t="n">
-        <v>297902.0</v>
+        <v>464732.0</v>
       </c>
       <c r="F6" s="8" t="n">
         <v>45020.0</v>
       </c>
       <c r="G6" s="9" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
       <c r="H6" s="10" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
     </row>
     <row r="7">
@@ -452,22 +452,22 @@
         </is>
       </c>
       <c r="C7" s="5" t="n">
-        <v>755012.0</v>
+        <v>734363.0</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>9438.6337890625</v>
+        <v>462756.9375</v>
       </c>
       <c r="E7" s="7" t="n">
-        <v>359439.0</v>
+        <v>62625.0</v>
       </c>
       <c r="F7" s="8" t="n">
         <v>45020.0</v>
       </c>
       <c r="G7" s="9" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
       <c r="H7" s="10" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
     </row>
     <row r="8">
@@ -482,22 +482,22 @@
         </is>
       </c>
       <c r="C8" s="5" t="n">
-        <v>277095.0</v>
+        <v>823141.0</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>198209.9375</v>
+        <v>361631.03125</v>
       </c>
       <c r="E8" s="7" t="n">
-        <v>742489.0</v>
+        <v>245904.0</v>
       </c>
       <c r="F8" s="8" t="n">
         <v>45020.0</v>
       </c>
       <c r="G8" s="9" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
       <c r="H8" s="10" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
     </row>
     <row r="9">
@@ -512,22 +512,22 @@
         </is>
       </c>
       <c r="C9" s="5" t="n">
-        <v>833938.0</v>
+        <v>409575.0</v>
       </c>
       <c r="D9" s="6" t="n">
-        <v>904344.6875</v>
+        <v>562065.9375</v>
       </c>
       <c r="E9" s="7" t="n">
-        <v>784051.0</v>
+        <v>629746.0</v>
       </c>
       <c r="F9" s="8" t="n">
         <v>45020.0</v>
       </c>
       <c r="G9" s="9" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
       <c r="H9" s="10" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
     </row>
     <row r="10">
@@ -542,22 +542,22 @@
         </is>
       </c>
       <c r="C10" s="5" t="n">
-        <v>428110.0</v>
+        <v>914266.0</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>763257.5</v>
+        <v>197526.8125</v>
       </c>
       <c r="E10" s="7" t="n">
-        <v>552668.0</v>
+        <v>455287.0</v>
       </c>
       <c r="F10" s="8" t="n">
         <v>45020.0</v>
       </c>
       <c r="G10" s="9" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
       <c r="H10" s="10" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
     </row>
     <row r="11">
@@ -572,22 +572,22 @@
         </is>
       </c>
       <c r="C11" s="5" t="n">
-        <v>183983.0</v>
+        <v>234904.0</v>
       </c>
       <c r="D11" s="6" t="n">
-        <v>813212.0625</v>
+        <v>928959.6875</v>
       </c>
       <c r="E11" s="7" t="n">
-        <v>24319.0</v>
+        <v>546612.0</v>
       </c>
       <c r="F11" s="8" t="n">
         <v>45020.0</v>
       </c>
       <c r="G11" s="9" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
       <c r="H11" s="10" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
     </row>
     <row r="12">
@@ -602,22 +602,22 @@
         </is>
       </c>
       <c r="C12" s="5" t="n">
-        <v>652746.0</v>
+        <v>792949.0</v>
       </c>
       <c r="D12" s="6" t="n">
-        <v>247624.34375</v>
+        <v>944007.25</v>
       </c>
       <c r="E12" s="7" t="n">
-        <v>164234.0</v>
+        <v>865461.0</v>
       </c>
       <c r="F12" s="8" t="n">
         <v>45020.0</v>
       </c>
       <c r="G12" s="9" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
       <c r="H12" s="10" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
     </row>
     <row r="13">
@@ -632,22 +632,22 @@
         </is>
       </c>
       <c r="C13" s="5" t="n">
-        <v>326721.0</v>
+        <v>509707.0</v>
       </c>
       <c r="D13" s="6" t="n">
-        <v>254885.375</v>
+        <v>625906.25</v>
       </c>
       <c r="E13" s="7" t="n">
-        <v>944602.0</v>
+        <v>917982.0</v>
       </c>
       <c r="F13" s="8" t="n">
         <v>45020.0</v>
       </c>
       <c r="G13" s="9" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
       <c r="H13" s="10" t="n">
-        <v>45020.68039681713</v>
+        <v>45020.69443405093</v>
       </c>
     </row>
   </sheetData>

</xml_diff>